<commit_message>
Date format convert issue fixed.
</commit_message>
<xml_diff>
--- a/asserts/ExcelFile.xlsx
+++ b/asserts/ExcelFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Sno</t>
   </si>
@@ -38,13 +38,19 @@
   </si>
   <si>
     <t>Raja</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy\ hh:mm"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +63,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -85,9 +102,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,15 +392,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="55.85546875" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +413,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -397,8 +427,11 @@
       <c r="C2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <v>41484.274791666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -408,8 +441,11 @@
       <c r="C3">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <v>41484.274791516204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -418,6 +454,9 @@
       </c>
       <c r="C4">
         <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>41484.274791516204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel file format updated.
</commit_message>
<xml_diff>
--- a/asserts/ExcelFile.xlsx
+++ b/asserts/ExcelFile.xlsx
@@ -48,7 +48,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm:ss.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -105,13 +105,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>